<commit_message>
WIP checkin (almost through to temp score)
WIP checkin...production/emission metrics still confused between types and dicts.

Signed-off-by: 72577720+MichaelTiemannOSC@users.noreply.github.com
Signed-off-by: MichaelTiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220927 ITR V2 Sample Data.xlsx
+++ b/examples/data/20220927 ITR V2 Sample Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/GitHub/ITR-MichaelTiemannOSC/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E93C148-8777-6745-ACDB-2258061F1D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B2DE2B-EA4D-D14E-9F96-CBD5758A2A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="6840" windowWidth="53580" windowHeight="26600" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7365,7 +7365,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H111" sqref="H111"/>
+      <selection pane="bottomRight" activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10683,8 +10683,14 @@
         <f>K109+K110</f>
         <v>1032498</v>
       </c>
-      <c r="L111" s="102"/>
-      <c r="M111" s="103"/>
+      <c r="L111" s="103">
+        <f>L109+L110</f>
+        <v>809057</v>
+      </c>
+      <c r="M111" s="103">
+        <f>M109+M110</f>
+        <v>834562</v>
+      </c>
     </row>
     <row r="112" spans="1:13">
       <c r="A112" s="116"/>
@@ -22819,69 +22825,162 @@
     </row>
   </sheetData>
   <mergeCells count="243">
-    <mergeCell ref="A109:A121"/>
-    <mergeCell ref="A31:A40"/>
-    <mergeCell ref="A122:A127"/>
-    <mergeCell ref="A128:A133"/>
-    <mergeCell ref="A134:A139"/>
-    <mergeCell ref="A140:A145"/>
-    <mergeCell ref="A146:A151"/>
-    <mergeCell ref="A152:A157"/>
-    <mergeCell ref="A158:A163"/>
-    <mergeCell ref="A164:A169"/>
-    <mergeCell ref="A170:A175"/>
-    <mergeCell ref="A176:A181"/>
-    <mergeCell ref="A182:A187"/>
-    <mergeCell ref="A188:A193"/>
-    <mergeCell ref="A194:A199"/>
-    <mergeCell ref="A200:A205"/>
-    <mergeCell ref="A206:A211"/>
-    <mergeCell ref="A212:A217"/>
-    <mergeCell ref="A218:A223"/>
-    <mergeCell ref="A224:A229"/>
-    <mergeCell ref="A230:A235"/>
-    <mergeCell ref="A236:A241"/>
-    <mergeCell ref="A242:A247"/>
-    <mergeCell ref="A248:A253"/>
-    <mergeCell ref="A254:A259"/>
-    <mergeCell ref="A260:A265"/>
-    <mergeCell ref="A266:A271"/>
-    <mergeCell ref="A272:A277"/>
-    <mergeCell ref="A278:A283"/>
-    <mergeCell ref="A284:A289"/>
-    <mergeCell ref="A290:A295"/>
-    <mergeCell ref="A296:A301"/>
-    <mergeCell ref="A302:A307"/>
-    <mergeCell ref="A308:A313"/>
-    <mergeCell ref="A314:A319"/>
-    <mergeCell ref="A320:A325"/>
-    <mergeCell ref="A326:A331"/>
-    <mergeCell ref="A332:A337"/>
-    <mergeCell ref="A338:A343"/>
-    <mergeCell ref="A344:A349"/>
-    <mergeCell ref="A350:A355"/>
-    <mergeCell ref="A356:A361"/>
-    <mergeCell ref="A362:A367"/>
-    <mergeCell ref="A368:A373"/>
-    <mergeCell ref="A374:A379"/>
-    <mergeCell ref="A380:A385"/>
-    <mergeCell ref="A386:A391"/>
-    <mergeCell ref="A392:A397"/>
-    <mergeCell ref="A398:A403"/>
-    <mergeCell ref="A404:A409"/>
-    <mergeCell ref="A410:A415"/>
-    <mergeCell ref="A416:A421"/>
-    <mergeCell ref="A422:A427"/>
-    <mergeCell ref="A428:A433"/>
-    <mergeCell ref="A434:A439"/>
-    <mergeCell ref="A440:A445"/>
-    <mergeCell ref="A446:A451"/>
-    <mergeCell ref="A452:A457"/>
-    <mergeCell ref="A458:A463"/>
-    <mergeCell ref="A464:A469"/>
-    <mergeCell ref="A470:A475"/>
-    <mergeCell ref="A476:A481"/>
-    <mergeCell ref="A482:A487"/>
+    <mergeCell ref="C512:C517"/>
+    <mergeCell ref="C518:C523"/>
+    <mergeCell ref="B31:B40"/>
+    <mergeCell ref="C31:C40"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="C11:C20"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="A96:A108"/>
+    <mergeCell ref="B96:B108"/>
+    <mergeCell ref="C96:C108"/>
+    <mergeCell ref="A83:A95"/>
+    <mergeCell ref="B83:B95"/>
+    <mergeCell ref="C83:C95"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="A71:A76"/>
+    <mergeCell ref="A77:A82"/>
+    <mergeCell ref="C458:C463"/>
+    <mergeCell ref="C464:C469"/>
+    <mergeCell ref="C470:C475"/>
+    <mergeCell ref="C476:C481"/>
+    <mergeCell ref="C482:C487"/>
+    <mergeCell ref="C488:C493"/>
+    <mergeCell ref="C494:C499"/>
+    <mergeCell ref="C500:C505"/>
+    <mergeCell ref="C506:C511"/>
+    <mergeCell ref="C404:C409"/>
+    <mergeCell ref="C410:C415"/>
+    <mergeCell ref="C416:C421"/>
+    <mergeCell ref="C422:C427"/>
+    <mergeCell ref="C428:C433"/>
+    <mergeCell ref="C434:C439"/>
+    <mergeCell ref="C440:C445"/>
+    <mergeCell ref="C446:C451"/>
+    <mergeCell ref="C452:C457"/>
+    <mergeCell ref="C350:C355"/>
+    <mergeCell ref="C356:C361"/>
+    <mergeCell ref="C362:C367"/>
+    <mergeCell ref="C368:C373"/>
+    <mergeCell ref="C374:C379"/>
+    <mergeCell ref="C380:C385"/>
+    <mergeCell ref="C386:C391"/>
+    <mergeCell ref="C392:C397"/>
+    <mergeCell ref="C398:C403"/>
+    <mergeCell ref="C296:C301"/>
+    <mergeCell ref="C302:C307"/>
+    <mergeCell ref="C308:C313"/>
+    <mergeCell ref="C314:C319"/>
+    <mergeCell ref="C320:C325"/>
+    <mergeCell ref="C326:C331"/>
+    <mergeCell ref="C332:C337"/>
+    <mergeCell ref="C338:C343"/>
+    <mergeCell ref="C344:C349"/>
+    <mergeCell ref="C242:C247"/>
+    <mergeCell ref="C248:C253"/>
+    <mergeCell ref="C254:C259"/>
+    <mergeCell ref="C260:C265"/>
+    <mergeCell ref="C266:C271"/>
+    <mergeCell ref="C272:C277"/>
+    <mergeCell ref="C278:C283"/>
+    <mergeCell ref="C284:C289"/>
+    <mergeCell ref="C290:C295"/>
+    <mergeCell ref="C188:C193"/>
+    <mergeCell ref="C194:C199"/>
+    <mergeCell ref="C200:C205"/>
+    <mergeCell ref="C206:C211"/>
+    <mergeCell ref="C212:C217"/>
+    <mergeCell ref="C218:C223"/>
+    <mergeCell ref="C224:C229"/>
+    <mergeCell ref="C230:C235"/>
+    <mergeCell ref="C236:C241"/>
+    <mergeCell ref="B500:B505"/>
+    <mergeCell ref="B506:B511"/>
+    <mergeCell ref="B512:B517"/>
+    <mergeCell ref="B518:B523"/>
+    <mergeCell ref="C21:C30"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="C59:C64"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="C77:C82"/>
+    <mergeCell ref="C109:C121"/>
+    <mergeCell ref="C122:C127"/>
+    <mergeCell ref="C128:C133"/>
+    <mergeCell ref="C134:C139"/>
+    <mergeCell ref="C140:C145"/>
+    <mergeCell ref="C146:C151"/>
+    <mergeCell ref="C152:C157"/>
+    <mergeCell ref="C158:C163"/>
+    <mergeCell ref="C164:C169"/>
+    <mergeCell ref="C170:C175"/>
+    <mergeCell ref="C176:C181"/>
+    <mergeCell ref="C182:C187"/>
+    <mergeCell ref="B446:B451"/>
+    <mergeCell ref="B452:B457"/>
+    <mergeCell ref="B458:B463"/>
+    <mergeCell ref="B464:B469"/>
+    <mergeCell ref="B470:B475"/>
+    <mergeCell ref="B476:B481"/>
+    <mergeCell ref="B482:B487"/>
+    <mergeCell ref="B488:B493"/>
+    <mergeCell ref="B494:B499"/>
+    <mergeCell ref="B392:B397"/>
+    <mergeCell ref="B398:B403"/>
+    <mergeCell ref="B404:B409"/>
+    <mergeCell ref="B410:B415"/>
+    <mergeCell ref="B416:B421"/>
+    <mergeCell ref="B422:B427"/>
+    <mergeCell ref="B428:B433"/>
+    <mergeCell ref="B434:B439"/>
+    <mergeCell ref="B440:B445"/>
+    <mergeCell ref="B338:B343"/>
+    <mergeCell ref="B344:B349"/>
+    <mergeCell ref="B350:B355"/>
+    <mergeCell ref="B356:B361"/>
+    <mergeCell ref="B362:B367"/>
+    <mergeCell ref="B368:B373"/>
+    <mergeCell ref="B374:B379"/>
+    <mergeCell ref="B380:B385"/>
+    <mergeCell ref="B386:B391"/>
+    <mergeCell ref="B284:B289"/>
+    <mergeCell ref="B290:B295"/>
+    <mergeCell ref="B296:B301"/>
+    <mergeCell ref="B302:B307"/>
+    <mergeCell ref="B308:B313"/>
+    <mergeCell ref="B314:B319"/>
+    <mergeCell ref="B320:B325"/>
+    <mergeCell ref="B326:B331"/>
+    <mergeCell ref="B332:B337"/>
+    <mergeCell ref="B230:B235"/>
+    <mergeCell ref="B236:B241"/>
+    <mergeCell ref="B242:B247"/>
+    <mergeCell ref="B248:B253"/>
+    <mergeCell ref="B254:B259"/>
+    <mergeCell ref="B260:B265"/>
+    <mergeCell ref="B266:B271"/>
+    <mergeCell ref="B272:B277"/>
+    <mergeCell ref="B278:B283"/>
+    <mergeCell ref="B176:B181"/>
+    <mergeCell ref="B182:B187"/>
+    <mergeCell ref="B188:B193"/>
+    <mergeCell ref="B194:B199"/>
+    <mergeCell ref="B200:B205"/>
+    <mergeCell ref="B206:B211"/>
+    <mergeCell ref="B212:B217"/>
+    <mergeCell ref="B218:B223"/>
+    <mergeCell ref="B224:B229"/>
     <mergeCell ref="A488:A493"/>
     <mergeCell ref="A494:A499"/>
     <mergeCell ref="A500:A505"/>
@@ -22906,162 +23005,69 @@
     <mergeCell ref="B158:B163"/>
     <mergeCell ref="B164:B169"/>
     <mergeCell ref="B170:B175"/>
-    <mergeCell ref="B176:B181"/>
-    <mergeCell ref="B182:B187"/>
-    <mergeCell ref="B188:B193"/>
-    <mergeCell ref="B194:B199"/>
-    <mergeCell ref="B200:B205"/>
-    <mergeCell ref="B206:B211"/>
-    <mergeCell ref="B212:B217"/>
-    <mergeCell ref="B218:B223"/>
-    <mergeCell ref="B224:B229"/>
-    <mergeCell ref="B230:B235"/>
-    <mergeCell ref="B236:B241"/>
-    <mergeCell ref="B242:B247"/>
-    <mergeCell ref="B248:B253"/>
-    <mergeCell ref="B254:B259"/>
-    <mergeCell ref="B260:B265"/>
-    <mergeCell ref="B266:B271"/>
-    <mergeCell ref="B272:B277"/>
-    <mergeCell ref="B278:B283"/>
-    <mergeCell ref="B284:B289"/>
-    <mergeCell ref="B290:B295"/>
-    <mergeCell ref="B296:B301"/>
-    <mergeCell ref="B302:B307"/>
-    <mergeCell ref="B308:B313"/>
-    <mergeCell ref="B314:B319"/>
-    <mergeCell ref="B320:B325"/>
-    <mergeCell ref="B326:B331"/>
-    <mergeCell ref="B332:B337"/>
-    <mergeCell ref="B338:B343"/>
-    <mergeCell ref="B344:B349"/>
-    <mergeCell ref="B350:B355"/>
-    <mergeCell ref="B356:B361"/>
-    <mergeCell ref="B362:B367"/>
-    <mergeCell ref="B368:B373"/>
-    <mergeCell ref="B374:B379"/>
-    <mergeCell ref="B380:B385"/>
-    <mergeCell ref="B386:B391"/>
-    <mergeCell ref="B392:B397"/>
-    <mergeCell ref="B398:B403"/>
-    <mergeCell ref="B404:B409"/>
-    <mergeCell ref="B410:B415"/>
-    <mergeCell ref="B416:B421"/>
-    <mergeCell ref="B422:B427"/>
-    <mergeCell ref="B428:B433"/>
-    <mergeCell ref="B434:B439"/>
-    <mergeCell ref="B440:B445"/>
-    <mergeCell ref="B446:B451"/>
-    <mergeCell ref="B452:B457"/>
-    <mergeCell ref="B458:B463"/>
-    <mergeCell ref="B464:B469"/>
-    <mergeCell ref="B470:B475"/>
-    <mergeCell ref="B476:B481"/>
-    <mergeCell ref="B482:B487"/>
-    <mergeCell ref="B488:B493"/>
-    <mergeCell ref="B494:B499"/>
-    <mergeCell ref="B500:B505"/>
-    <mergeCell ref="B506:B511"/>
-    <mergeCell ref="B512:B517"/>
-    <mergeCell ref="B518:B523"/>
-    <mergeCell ref="C21:C30"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="C59:C64"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="C77:C82"/>
-    <mergeCell ref="C109:C121"/>
-    <mergeCell ref="C122:C127"/>
-    <mergeCell ref="C128:C133"/>
-    <mergeCell ref="C134:C139"/>
-    <mergeCell ref="C140:C145"/>
-    <mergeCell ref="C146:C151"/>
-    <mergeCell ref="C152:C157"/>
-    <mergeCell ref="C158:C163"/>
-    <mergeCell ref="C164:C169"/>
-    <mergeCell ref="C170:C175"/>
-    <mergeCell ref="C176:C181"/>
-    <mergeCell ref="C182:C187"/>
-    <mergeCell ref="C188:C193"/>
-    <mergeCell ref="C194:C199"/>
-    <mergeCell ref="C200:C205"/>
-    <mergeCell ref="C206:C211"/>
-    <mergeCell ref="C212:C217"/>
-    <mergeCell ref="C218:C223"/>
-    <mergeCell ref="C224:C229"/>
-    <mergeCell ref="C230:C235"/>
-    <mergeCell ref="C236:C241"/>
-    <mergeCell ref="C242:C247"/>
-    <mergeCell ref="C248:C253"/>
-    <mergeCell ref="C254:C259"/>
-    <mergeCell ref="C260:C265"/>
-    <mergeCell ref="C266:C271"/>
-    <mergeCell ref="C272:C277"/>
-    <mergeCell ref="C278:C283"/>
-    <mergeCell ref="C284:C289"/>
-    <mergeCell ref="C290:C295"/>
-    <mergeCell ref="C296:C301"/>
-    <mergeCell ref="C302:C307"/>
-    <mergeCell ref="C308:C313"/>
-    <mergeCell ref="C314:C319"/>
-    <mergeCell ref="C320:C325"/>
-    <mergeCell ref="C326:C331"/>
-    <mergeCell ref="C332:C337"/>
-    <mergeCell ref="C338:C343"/>
-    <mergeCell ref="C344:C349"/>
-    <mergeCell ref="C350:C355"/>
-    <mergeCell ref="C356:C361"/>
-    <mergeCell ref="C362:C367"/>
-    <mergeCell ref="C368:C373"/>
-    <mergeCell ref="C374:C379"/>
-    <mergeCell ref="C380:C385"/>
-    <mergeCell ref="C386:C391"/>
-    <mergeCell ref="C392:C397"/>
-    <mergeCell ref="C398:C403"/>
-    <mergeCell ref="C404:C409"/>
-    <mergeCell ref="C410:C415"/>
-    <mergeCell ref="C416:C421"/>
-    <mergeCell ref="C422:C427"/>
-    <mergeCell ref="C428:C433"/>
-    <mergeCell ref="C434:C439"/>
-    <mergeCell ref="C440:C445"/>
-    <mergeCell ref="C446:C451"/>
-    <mergeCell ref="C452:C457"/>
-    <mergeCell ref="C458:C463"/>
-    <mergeCell ref="C464:C469"/>
-    <mergeCell ref="C470:C475"/>
-    <mergeCell ref="C476:C481"/>
-    <mergeCell ref="C482:C487"/>
-    <mergeCell ref="C488:C493"/>
-    <mergeCell ref="C494:C499"/>
-    <mergeCell ref="C500:C505"/>
-    <mergeCell ref="C506:C511"/>
-    <mergeCell ref="C512:C517"/>
-    <mergeCell ref="C518:C523"/>
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="C31:C40"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="B11:B20"/>
-    <mergeCell ref="C11:C20"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="A96:A108"/>
-    <mergeCell ref="B96:B108"/>
-    <mergeCell ref="C96:C108"/>
-    <mergeCell ref="A83:A95"/>
-    <mergeCell ref="B83:B95"/>
-    <mergeCell ref="C83:C95"/>
-    <mergeCell ref="A21:A30"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="A77:A82"/>
+    <mergeCell ref="A434:A439"/>
+    <mergeCell ref="A440:A445"/>
+    <mergeCell ref="A446:A451"/>
+    <mergeCell ref="A452:A457"/>
+    <mergeCell ref="A458:A463"/>
+    <mergeCell ref="A464:A469"/>
+    <mergeCell ref="A470:A475"/>
+    <mergeCell ref="A476:A481"/>
+    <mergeCell ref="A482:A487"/>
+    <mergeCell ref="A380:A385"/>
+    <mergeCell ref="A386:A391"/>
+    <mergeCell ref="A392:A397"/>
+    <mergeCell ref="A398:A403"/>
+    <mergeCell ref="A404:A409"/>
+    <mergeCell ref="A410:A415"/>
+    <mergeCell ref="A416:A421"/>
+    <mergeCell ref="A422:A427"/>
+    <mergeCell ref="A428:A433"/>
+    <mergeCell ref="A326:A331"/>
+    <mergeCell ref="A332:A337"/>
+    <mergeCell ref="A338:A343"/>
+    <mergeCell ref="A344:A349"/>
+    <mergeCell ref="A350:A355"/>
+    <mergeCell ref="A356:A361"/>
+    <mergeCell ref="A362:A367"/>
+    <mergeCell ref="A368:A373"/>
+    <mergeCell ref="A374:A379"/>
+    <mergeCell ref="A272:A277"/>
+    <mergeCell ref="A278:A283"/>
+    <mergeCell ref="A284:A289"/>
+    <mergeCell ref="A290:A295"/>
+    <mergeCell ref="A296:A301"/>
+    <mergeCell ref="A302:A307"/>
+    <mergeCell ref="A308:A313"/>
+    <mergeCell ref="A314:A319"/>
+    <mergeCell ref="A320:A325"/>
+    <mergeCell ref="A218:A223"/>
+    <mergeCell ref="A224:A229"/>
+    <mergeCell ref="A230:A235"/>
+    <mergeCell ref="A236:A241"/>
+    <mergeCell ref="A242:A247"/>
+    <mergeCell ref="A248:A253"/>
+    <mergeCell ref="A254:A259"/>
+    <mergeCell ref="A260:A265"/>
+    <mergeCell ref="A266:A271"/>
+    <mergeCell ref="A164:A169"/>
+    <mergeCell ref="A170:A175"/>
+    <mergeCell ref="A176:A181"/>
+    <mergeCell ref="A182:A187"/>
+    <mergeCell ref="A188:A193"/>
+    <mergeCell ref="A194:A199"/>
+    <mergeCell ref="A200:A205"/>
+    <mergeCell ref="A206:A211"/>
+    <mergeCell ref="A212:A217"/>
+    <mergeCell ref="A109:A121"/>
+    <mergeCell ref="A31:A40"/>
+    <mergeCell ref="A122:A127"/>
+    <mergeCell ref="A128:A133"/>
+    <mergeCell ref="A134:A139"/>
+    <mergeCell ref="A140:A145"/>
+    <mergeCell ref="A146:A151"/>
+    <mergeCell ref="A152:A157"/>
+    <mergeCell ref="A158:A163"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L30" r:id="rId1" xr:uid="{0B00E541-600E-124F-8530-7CF03623D698}"/>
@@ -38699,7 +38705,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E33" ca="1" si="0">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>222587708</v>
+        <v>53807700</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -38717,7 +38723,7 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>202902030</v>
+        <v>181209960</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -38735,7 +38741,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>37756880</v>
+        <v>223089968</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -38753,7 +38759,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>146973042</v>
+        <v>78534720</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -38771,7 +38777,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>240779433</v>
+        <v>80120240</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -38789,7 +38795,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>188394765</v>
+        <v>165312707</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -38807,7 +38813,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>59522814</v>
+        <v>139146044</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -38825,7 +38831,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>50230292</v>
+        <v>56760876</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -38843,7 +38849,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>143602465</v>
+        <v>89155408</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -38861,7 +38867,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>171004750</v>
+        <v>111742680</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -38879,7 +38885,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>100991820</v>
+        <v>158968084</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -38897,7 +38903,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>79908452</v>
+        <v>94129060</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -38915,7 +38921,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>62183640</v>
+        <v>97145860</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -38933,7 +38939,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>225538950</v>
+        <v>87841455</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -38951,7 +38957,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>134965320</v>
+        <v>240109632</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -38969,7 +38975,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>173578563</v>
+        <v>195168402</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -38987,7 +38993,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>148352254</v>
+        <v>173944316</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -39005,7 +39011,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>95075977</v>
+        <v>72882801</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -39023,7 +39029,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>139777386</v>
+        <v>123364408</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -39041,7 +39047,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>81976488</v>
+        <v>54345746</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -39059,7 +39065,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>159383748</v>
+        <v>190230397</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -39077,7 +39083,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>84671118</v>
+        <v>168419412</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -39095,7 +39101,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>152181897</v>
+        <v>57811131</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -39113,7 +39119,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>170292096</v>
+        <v>86247408</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -39131,7 +39137,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>147779541</v>
+        <v>263152125</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -39149,7 +39155,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>52182423</v>
+        <v>105507432</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -39167,7 +39173,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>148477968</v>
+        <v>53306856</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -39185,7 +39191,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>78579858</v>
+        <v>74529563</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -39203,7 +39209,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>87121775</v>
+        <v>204601320</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -39221,7 +39227,7 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>154820064</v>
+        <v>85736835</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -39239,7 +39245,7 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>49996941</v>
+        <v>177301980</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -39257,7 +39263,7 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>168110487</v>
+        <v>162051120</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -39275,7 +39281,7 @@
       </c>
       <c r="E34">
         <f t="shared" ref="E34:E65" ca="1" si="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>260415748</v>
+        <v>142147460</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -39293,7 +39299,7 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="1"/>
-        <v>125891616</v>
+        <v>90356789</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -39311,7 +39317,7 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="1"/>
-        <v>99585864</v>
+        <v>75372750</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -39329,7 +39335,7 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="1"/>
-        <v>117109244</v>
+        <v>236009256</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -39347,7 +39353,7 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="1"/>
-        <v>41629110</v>
+        <v>89950768</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -39365,7 +39371,7 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="1"/>
-        <v>167340508</v>
+        <v>110745240</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -39383,7 +39389,7 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="1"/>
-        <v>68834921</v>
+        <v>185294325</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -39401,7 +39407,7 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="1"/>
-        <v>54207021</v>
+        <v>134619111</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -39419,7 +39425,7 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="1"/>
-        <v>157929184</v>
+        <v>212122612</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -39437,7 +39443,7 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="1"/>
-        <v>165328052</v>
+        <v>138767648</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -39455,7 +39461,7 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="1"/>
-        <v>158034732</v>
+        <v>88706457</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -39473,7 +39479,7 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="1"/>
-        <v>80534293</v>
+        <v>78461328</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -39491,7 +39497,7 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="1"/>
-        <v>144363222</v>
+        <v>58904592</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -39509,7 +39515,7 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="1"/>
-        <v>191311860</v>
+        <v>46117565</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -39527,7 +39533,7 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="1"/>
-        <v>124624170</v>
+        <v>41545819</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -39545,7 +39551,7 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="1"/>
-        <v>54760992</v>
+        <v>135474649</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -39563,7 +39569,7 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="1"/>
-        <v>159231526</v>
+        <v>194834304</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -39581,7 +39587,7 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="1"/>
-        <v>132468049</v>
+        <v>243317382</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -39599,7 +39605,7 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="1"/>
-        <v>130938552</v>
+        <v>172638588</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -39617,7 +39623,7 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="1"/>
-        <v>126329712</v>
+        <v>201195954</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -39635,7 +39641,7 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="1"/>
-        <v>292065480</v>
+        <v>264227990</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -39653,7 +39659,7 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="1"/>
-        <v>168725952</v>
+        <v>112045038</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -39671,7 +39677,7 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="1"/>
-        <v>94209800</v>
+        <v>157112634</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -39689,7 +39695,7 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="1"/>
-        <v>240084000</v>
+        <v>49154235</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -39707,7 +39713,7 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="1"/>
-        <v>84229800</v>
+        <v>158965521</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -39725,7 +39731,7 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="1"/>
-        <v>241851799</v>
+        <v>72738699</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -39743,7 +39749,7 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="1"/>
-        <v>57684838</v>
+        <v>199525529</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -39761,7 +39767,7 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="1"/>
-        <v>208946400</v>
+        <v>192131433</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -39779,7 +39785,7 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="1"/>
-        <v>77123310</v>
+        <v>173485528</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -39797,7 +39803,7 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="1"/>
-        <v>247614628</v>
+        <v>53507430</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -39815,7 +39821,7 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="1"/>
-        <v>65678704</v>
+        <v>244184005</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -39833,7 +39839,7 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="1"/>
-        <v>204792074</v>
+        <v>39726207</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -39851,7 +39857,7 @@
       </c>
       <c r="E66">
         <f t="shared" ref="E66:E77" ca="1" si="2">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>229314564</v>
+        <v>170594082</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -39869,7 +39875,7 @@
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="2"/>
-        <v>194720094</v>
+        <v>149704495</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -39887,7 +39893,7 @@
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="2"/>
-        <v>166396778</v>
+        <v>132802620</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -39905,7 +39911,7 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="2"/>
-        <v>186117720</v>
+        <v>146999628</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -39923,7 +39929,7 @@
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="2"/>
-        <v>66843090</v>
+        <v>166414070</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -39941,7 +39947,7 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="2"/>
-        <v>114058848</v>
+        <v>175784764</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -39959,7 +39965,7 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="2"/>
-        <v>217846845</v>
+        <v>122850660</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -39977,7 +39983,7 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="2"/>
-        <v>166425996</v>
+        <v>41995944</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -39995,7 +40001,7 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="2"/>
-        <v>115861039</v>
+        <v>47755008</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -40013,7 +40019,7 @@
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="2"/>
-        <v>63698490</v>
+        <v>62139792</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -40031,7 +40037,7 @@
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="2"/>
-        <v>156961722</v>
+        <v>116744285</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -40049,7 +40055,7 @@
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="2"/>
-        <v>60225659</v>
+        <v>183501214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 8 sectors * 3 regions
Change name of "Oil & Gas" sector to "Energy" and add three energy sub-sectors (Coal, Oil, Gas).  Also add 5 chemical subsectors, fixing unit conversions exposed as needing help.

Update recent sample data accordingly.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20220927 ITR V2 Sample Data.xlsx
+++ b/examples/data/20220927 ITR V2 Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Dropbox/My Mac (MacBook-Pro.local)/Documents/GitHub/MichaelTiemannOSC/ITR/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ECEA55-CBAC-9A4A-8107-058DA24CBF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB80E614-3251-F640-87B1-376F431FF9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20740" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4320" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4320" uniqueCount="463">
   <si>
     <t>company_name</t>
   </si>
@@ -1841,6 +1841,9 @@
   </si>
   <si>
     <t>submetric</t>
+  </si>
+  <si>
+    <t>Energy</t>
   </si>
 </sst>
 </file>
@@ -3685,7 +3688,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -4183,7 +4188,7 @@
         <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G11" t="s">
         <v>56</v>
@@ -4275,7 +4280,7 @@
       </c>
       <c r="E13" s="94"/>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G13" t="s">
         <v>56</v>
@@ -5025,7 +5030,7 @@
         <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G29" t="s">
         <v>56</v>
@@ -5391,7 +5396,7 @@
       </c>
       <c r="E37" s="94"/>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G37" t="s">
         <v>56</v>
@@ -5810,7 +5815,7 @@
       </c>
       <c r="E46" s="94"/>
       <c r="F46" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G46" t="s">
         <v>56</v>
@@ -5855,7 +5860,7 @@
       </c>
       <c r="E47" s="94"/>
       <c r="F47" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G47" t="s">
         <v>56</v>
@@ -6229,7 +6234,7 @@
       </c>
       <c r="E55" s="94"/>
       <c r="F55" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G55" t="s">
         <v>56</v>
@@ -6323,7 +6328,7 @@
         <v>95</v>
       </c>
       <c r="F57" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G57" t="s">
         <v>56</v>
@@ -6368,7 +6373,7 @@
       </c>
       <c r="E58" s="94"/>
       <c r="F58" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G58" t="s">
         <v>56</v>
@@ -6413,7 +6418,7 @@
       </c>
       <c r="E59" s="94"/>
       <c r="F59" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
       <c r="G59" t="s">
         <v>56</v>
@@ -7290,7 +7295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M523"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -22451,69 +22456,162 @@
     </row>
   </sheetData>
   <mergeCells count="243">
-    <mergeCell ref="A109:A121"/>
-    <mergeCell ref="A31:A40"/>
-    <mergeCell ref="A122:A127"/>
-    <mergeCell ref="A128:A133"/>
-    <mergeCell ref="A134:A139"/>
-    <mergeCell ref="A140:A145"/>
-    <mergeCell ref="A146:A151"/>
-    <mergeCell ref="A152:A157"/>
-    <mergeCell ref="A158:A163"/>
-    <mergeCell ref="A164:A169"/>
-    <mergeCell ref="A170:A175"/>
-    <mergeCell ref="A176:A181"/>
-    <mergeCell ref="A182:A187"/>
-    <mergeCell ref="A188:A193"/>
-    <mergeCell ref="A194:A199"/>
-    <mergeCell ref="A200:A205"/>
-    <mergeCell ref="A206:A211"/>
-    <mergeCell ref="A212:A217"/>
-    <mergeCell ref="A218:A223"/>
-    <mergeCell ref="A224:A229"/>
-    <mergeCell ref="A230:A235"/>
-    <mergeCell ref="A236:A241"/>
-    <mergeCell ref="A242:A247"/>
-    <mergeCell ref="A248:A253"/>
-    <mergeCell ref="A254:A259"/>
-    <mergeCell ref="A260:A265"/>
-    <mergeCell ref="A266:A271"/>
-    <mergeCell ref="A272:A277"/>
-    <mergeCell ref="A278:A283"/>
-    <mergeCell ref="A284:A289"/>
-    <mergeCell ref="A290:A295"/>
-    <mergeCell ref="A296:A301"/>
-    <mergeCell ref="A302:A307"/>
-    <mergeCell ref="A308:A313"/>
-    <mergeCell ref="A314:A319"/>
-    <mergeCell ref="A320:A325"/>
-    <mergeCell ref="A326:A331"/>
-    <mergeCell ref="A332:A337"/>
-    <mergeCell ref="A338:A343"/>
-    <mergeCell ref="A344:A349"/>
-    <mergeCell ref="A350:A355"/>
-    <mergeCell ref="A356:A361"/>
-    <mergeCell ref="A362:A367"/>
-    <mergeCell ref="A368:A373"/>
-    <mergeCell ref="A374:A379"/>
-    <mergeCell ref="A380:A385"/>
-    <mergeCell ref="A386:A391"/>
-    <mergeCell ref="A392:A397"/>
-    <mergeCell ref="A398:A403"/>
-    <mergeCell ref="A404:A409"/>
-    <mergeCell ref="A410:A415"/>
-    <mergeCell ref="A416:A421"/>
-    <mergeCell ref="A422:A427"/>
-    <mergeCell ref="A428:A433"/>
-    <mergeCell ref="A434:A439"/>
-    <mergeCell ref="A440:A445"/>
-    <mergeCell ref="A446:A451"/>
-    <mergeCell ref="A452:A457"/>
-    <mergeCell ref="A458:A463"/>
-    <mergeCell ref="A464:A469"/>
-    <mergeCell ref="A470:A475"/>
-    <mergeCell ref="A476:A481"/>
-    <mergeCell ref="A482:A487"/>
+    <mergeCell ref="C512:C517"/>
+    <mergeCell ref="C518:C523"/>
+    <mergeCell ref="B31:B40"/>
+    <mergeCell ref="C31:C40"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="C11:C20"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="A96:A108"/>
+    <mergeCell ref="B96:B108"/>
+    <mergeCell ref="C96:C108"/>
+    <mergeCell ref="A83:A95"/>
+    <mergeCell ref="B83:B95"/>
+    <mergeCell ref="C83:C95"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="A59:A64"/>
+    <mergeCell ref="A65:A70"/>
+    <mergeCell ref="A71:A76"/>
+    <mergeCell ref="A77:A82"/>
+    <mergeCell ref="C458:C463"/>
+    <mergeCell ref="C464:C469"/>
+    <mergeCell ref="C470:C475"/>
+    <mergeCell ref="C476:C481"/>
+    <mergeCell ref="C482:C487"/>
+    <mergeCell ref="C488:C493"/>
+    <mergeCell ref="C494:C499"/>
+    <mergeCell ref="C500:C505"/>
+    <mergeCell ref="C506:C511"/>
+    <mergeCell ref="C404:C409"/>
+    <mergeCell ref="C410:C415"/>
+    <mergeCell ref="C416:C421"/>
+    <mergeCell ref="C422:C427"/>
+    <mergeCell ref="C428:C433"/>
+    <mergeCell ref="C434:C439"/>
+    <mergeCell ref="C440:C445"/>
+    <mergeCell ref="C446:C451"/>
+    <mergeCell ref="C452:C457"/>
+    <mergeCell ref="C350:C355"/>
+    <mergeCell ref="C356:C361"/>
+    <mergeCell ref="C362:C367"/>
+    <mergeCell ref="C368:C373"/>
+    <mergeCell ref="C374:C379"/>
+    <mergeCell ref="C380:C385"/>
+    <mergeCell ref="C386:C391"/>
+    <mergeCell ref="C392:C397"/>
+    <mergeCell ref="C398:C403"/>
+    <mergeCell ref="C296:C301"/>
+    <mergeCell ref="C302:C307"/>
+    <mergeCell ref="C308:C313"/>
+    <mergeCell ref="C314:C319"/>
+    <mergeCell ref="C320:C325"/>
+    <mergeCell ref="C326:C331"/>
+    <mergeCell ref="C332:C337"/>
+    <mergeCell ref="C338:C343"/>
+    <mergeCell ref="C344:C349"/>
+    <mergeCell ref="C242:C247"/>
+    <mergeCell ref="C248:C253"/>
+    <mergeCell ref="C254:C259"/>
+    <mergeCell ref="C260:C265"/>
+    <mergeCell ref="C266:C271"/>
+    <mergeCell ref="C272:C277"/>
+    <mergeCell ref="C278:C283"/>
+    <mergeCell ref="C284:C289"/>
+    <mergeCell ref="C290:C295"/>
+    <mergeCell ref="C188:C193"/>
+    <mergeCell ref="C194:C199"/>
+    <mergeCell ref="C200:C205"/>
+    <mergeCell ref="C206:C211"/>
+    <mergeCell ref="C212:C217"/>
+    <mergeCell ref="C218:C223"/>
+    <mergeCell ref="C224:C229"/>
+    <mergeCell ref="C230:C235"/>
+    <mergeCell ref="C236:C241"/>
+    <mergeCell ref="B500:B505"/>
+    <mergeCell ref="B506:B511"/>
+    <mergeCell ref="B512:B517"/>
+    <mergeCell ref="B518:B523"/>
+    <mergeCell ref="C21:C30"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="C59:C64"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="C77:C82"/>
+    <mergeCell ref="C109:C121"/>
+    <mergeCell ref="C122:C127"/>
+    <mergeCell ref="C128:C133"/>
+    <mergeCell ref="C134:C139"/>
+    <mergeCell ref="C140:C145"/>
+    <mergeCell ref="C146:C151"/>
+    <mergeCell ref="C152:C157"/>
+    <mergeCell ref="C158:C163"/>
+    <mergeCell ref="C164:C169"/>
+    <mergeCell ref="C170:C175"/>
+    <mergeCell ref="C176:C181"/>
+    <mergeCell ref="C182:C187"/>
+    <mergeCell ref="B446:B451"/>
+    <mergeCell ref="B452:B457"/>
+    <mergeCell ref="B458:B463"/>
+    <mergeCell ref="B464:B469"/>
+    <mergeCell ref="B470:B475"/>
+    <mergeCell ref="B476:B481"/>
+    <mergeCell ref="B482:B487"/>
+    <mergeCell ref="B488:B493"/>
+    <mergeCell ref="B494:B499"/>
+    <mergeCell ref="B392:B397"/>
+    <mergeCell ref="B398:B403"/>
+    <mergeCell ref="B404:B409"/>
+    <mergeCell ref="B410:B415"/>
+    <mergeCell ref="B416:B421"/>
+    <mergeCell ref="B422:B427"/>
+    <mergeCell ref="B428:B433"/>
+    <mergeCell ref="B434:B439"/>
+    <mergeCell ref="B440:B445"/>
+    <mergeCell ref="B338:B343"/>
+    <mergeCell ref="B344:B349"/>
+    <mergeCell ref="B350:B355"/>
+    <mergeCell ref="B356:B361"/>
+    <mergeCell ref="B362:B367"/>
+    <mergeCell ref="B368:B373"/>
+    <mergeCell ref="B374:B379"/>
+    <mergeCell ref="B380:B385"/>
+    <mergeCell ref="B386:B391"/>
+    <mergeCell ref="B284:B289"/>
+    <mergeCell ref="B290:B295"/>
+    <mergeCell ref="B296:B301"/>
+    <mergeCell ref="B302:B307"/>
+    <mergeCell ref="B308:B313"/>
+    <mergeCell ref="B314:B319"/>
+    <mergeCell ref="B320:B325"/>
+    <mergeCell ref="B326:B331"/>
+    <mergeCell ref="B332:B337"/>
+    <mergeCell ref="B230:B235"/>
+    <mergeCell ref="B236:B241"/>
+    <mergeCell ref="B242:B247"/>
+    <mergeCell ref="B248:B253"/>
+    <mergeCell ref="B254:B259"/>
+    <mergeCell ref="B260:B265"/>
+    <mergeCell ref="B266:B271"/>
+    <mergeCell ref="B272:B277"/>
+    <mergeCell ref="B278:B283"/>
+    <mergeCell ref="B176:B181"/>
+    <mergeCell ref="B182:B187"/>
+    <mergeCell ref="B188:B193"/>
+    <mergeCell ref="B194:B199"/>
+    <mergeCell ref="B200:B205"/>
+    <mergeCell ref="B206:B211"/>
+    <mergeCell ref="B212:B217"/>
+    <mergeCell ref="B218:B223"/>
+    <mergeCell ref="B224:B229"/>
     <mergeCell ref="A488:A493"/>
     <mergeCell ref="A494:A499"/>
     <mergeCell ref="A500:A505"/>
@@ -22538,162 +22636,69 @@
     <mergeCell ref="B158:B163"/>
     <mergeCell ref="B164:B169"/>
     <mergeCell ref="B170:B175"/>
-    <mergeCell ref="B176:B181"/>
-    <mergeCell ref="B182:B187"/>
-    <mergeCell ref="B188:B193"/>
-    <mergeCell ref="B194:B199"/>
-    <mergeCell ref="B200:B205"/>
-    <mergeCell ref="B206:B211"/>
-    <mergeCell ref="B212:B217"/>
-    <mergeCell ref="B218:B223"/>
-    <mergeCell ref="B224:B229"/>
-    <mergeCell ref="B230:B235"/>
-    <mergeCell ref="B236:B241"/>
-    <mergeCell ref="B242:B247"/>
-    <mergeCell ref="B248:B253"/>
-    <mergeCell ref="B254:B259"/>
-    <mergeCell ref="B260:B265"/>
-    <mergeCell ref="B266:B271"/>
-    <mergeCell ref="B272:B277"/>
-    <mergeCell ref="B278:B283"/>
-    <mergeCell ref="B284:B289"/>
-    <mergeCell ref="B290:B295"/>
-    <mergeCell ref="B296:B301"/>
-    <mergeCell ref="B302:B307"/>
-    <mergeCell ref="B308:B313"/>
-    <mergeCell ref="B314:B319"/>
-    <mergeCell ref="B320:B325"/>
-    <mergeCell ref="B326:B331"/>
-    <mergeCell ref="B332:B337"/>
-    <mergeCell ref="B338:B343"/>
-    <mergeCell ref="B344:B349"/>
-    <mergeCell ref="B350:B355"/>
-    <mergeCell ref="B356:B361"/>
-    <mergeCell ref="B362:B367"/>
-    <mergeCell ref="B368:B373"/>
-    <mergeCell ref="B374:B379"/>
-    <mergeCell ref="B380:B385"/>
-    <mergeCell ref="B386:B391"/>
-    <mergeCell ref="B392:B397"/>
-    <mergeCell ref="B398:B403"/>
-    <mergeCell ref="B404:B409"/>
-    <mergeCell ref="B410:B415"/>
-    <mergeCell ref="B416:B421"/>
-    <mergeCell ref="B422:B427"/>
-    <mergeCell ref="B428:B433"/>
-    <mergeCell ref="B434:B439"/>
-    <mergeCell ref="B440:B445"/>
-    <mergeCell ref="B446:B451"/>
-    <mergeCell ref="B452:B457"/>
-    <mergeCell ref="B458:B463"/>
-    <mergeCell ref="B464:B469"/>
-    <mergeCell ref="B470:B475"/>
-    <mergeCell ref="B476:B481"/>
-    <mergeCell ref="B482:B487"/>
-    <mergeCell ref="B488:B493"/>
-    <mergeCell ref="B494:B499"/>
-    <mergeCell ref="B500:B505"/>
-    <mergeCell ref="B506:B511"/>
-    <mergeCell ref="B512:B517"/>
-    <mergeCell ref="B518:B523"/>
-    <mergeCell ref="C21:C30"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="C59:C64"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="C77:C82"/>
-    <mergeCell ref="C109:C121"/>
-    <mergeCell ref="C122:C127"/>
-    <mergeCell ref="C128:C133"/>
-    <mergeCell ref="C134:C139"/>
-    <mergeCell ref="C140:C145"/>
-    <mergeCell ref="C146:C151"/>
-    <mergeCell ref="C152:C157"/>
-    <mergeCell ref="C158:C163"/>
-    <mergeCell ref="C164:C169"/>
-    <mergeCell ref="C170:C175"/>
-    <mergeCell ref="C176:C181"/>
-    <mergeCell ref="C182:C187"/>
-    <mergeCell ref="C188:C193"/>
-    <mergeCell ref="C194:C199"/>
-    <mergeCell ref="C200:C205"/>
-    <mergeCell ref="C206:C211"/>
-    <mergeCell ref="C212:C217"/>
-    <mergeCell ref="C218:C223"/>
-    <mergeCell ref="C224:C229"/>
-    <mergeCell ref="C230:C235"/>
-    <mergeCell ref="C236:C241"/>
-    <mergeCell ref="C242:C247"/>
-    <mergeCell ref="C248:C253"/>
-    <mergeCell ref="C254:C259"/>
-    <mergeCell ref="C260:C265"/>
-    <mergeCell ref="C266:C271"/>
-    <mergeCell ref="C272:C277"/>
-    <mergeCell ref="C278:C283"/>
-    <mergeCell ref="C284:C289"/>
-    <mergeCell ref="C290:C295"/>
-    <mergeCell ref="C296:C301"/>
-    <mergeCell ref="C302:C307"/>
-    <mergeCell ref="C308:C313"/>
-    <mergeCell ref="C314:C319"/>
-    <mergeCell ref="C320:C325"/>
-    <mergeCell ref="C326:C331"/>
-    <mergeCell ref="C332:C337"/>
-    <mergeCell ref="C338:C343"/>
-    <mergeCell ref="C344:C349"/>
-    <mergeCell ref="C350:C355"/>
-    <mergeCell ref="C356:C361"/>
-    <mergeCell ref="C362:C367"/>
-    <mergeCell ref="C368:C373"/>
-    <mergeCell ref="C374:C379"/>
-    <mergeCell ref="C380:C385"/>
-    <mergeCell ref="C386:C391"/>
-    <mergeCell ref="C392:C397"/>
-    <mergeCell ref="C398:C403"/>
-    <mergeCell ref="C404:C409"/>
-    <mergeCell ref="C410:C415"/>
-    <mergeCell ref="C416:C421"/>
-    <mergeCell ref="C422:C427"/>
-    <mergeCell ref="C428:C433"/>
-    <mergeCell ref="C434:C439"/>
-    <mergeCell ref="C440:C445"/>
-    <mergeCell ref="C446:C451"/>
-    <mergeCell ref="C452:C457"/>
-    <mergeCell ref="C458:C463"/>
-    <mergeCell ref="C464:C469"/>
-    <mergeCell ref="C470:C475"/>
-    <mergeCell ref="C476:C481"/>
-    <mergeCell ref="C482:C487"/>
-    <mergeCell ref="C488:C493"/>
-    <mergeCell ref="C494:C499"/>
-    <mergeCell ref="C500:C505"/>
-    <mergeCell ref="C506:C511"/>
-    <mergeCell ref="C512:C517"/>
-    <mergeCell ref="C518:C523"/>
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="C31:C40"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="B11:B20"/>
-    <mergeCell ref="C11:C20"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="A96:A108"/>
-    <mergeCell ref="B96:B108"/>
-    <mergeCell ref="C96:C108"/>
-    <mergeCell ref="A83:A95"/>
-    <mergeCell ref="B83:B95"/>
-    <mergeCell ref="C83:C95"/>
-    <mergeCell ref="A21:A30"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:A52"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="A65:A70"/>
-    <mergeCell ref="A71:A76"/>
-    <mergeCell ref="A77:A82"/>
+    <mergeCell ref="A434:A439"/>
+    <mergeCell ref="A440:A445"/>
+    <mergeCell ref="A446:A451"/>
+    <mergeCell ref="A452:A457"/>
+    <mergeCell ref="A458:A463"/>
+    <mergeCell ref="A464:A469"/>
+    <mergeCell ref="A470:A475"/>
+    <mergeCell ref="A476:A481"/>
+    <mergeCell ref="A482:A487"/>
+    <mergeCell ref="A380:A385"/>
+    <mergeCell ref="A386:A391"/>
+    <mergeCell ref="A392:A397"/>
+    <mergeCell ref="A398:A403"/>
+    <mergeCell ref="A404:A409"/>
+    <mergeCell ref="A410:A415"/>
+    <mergeCell ref="A416:A421"/>
+    <mergeCell ref="A422:A427"/>
+    <mergeCell ref="A428:A433"/>
+    <mergeCell ref="A326:A331"/>
+    <mergeCell ref="A332:A337"/>
+    <mergeCell ref="A338:A343"/>
+    <mergeCell ref="A344:A349"/>
+    <mergeCell ref="A350:A355"/>
+    <mergeCell ref="A356:A361"/>
+    <mergeCell ref="A362:A367"/>
+    <mergeCell ref="A368:A373"/>
+    <mergeCell ref="A374:A379"/>
+    <mergeCell ref="A272:A277"/>
+    <mergeCell ref="A278:A283"/>
+    <mergeCell ref="A284:A289"/>
+    <mergeCell ref="A290:A295"/>
+    <mergeCell ref="A296:A301"/>
+    <mergeCell ref="A302:A307"/>
+    <mergeCell ref="A308:A313"/>
+    <mergeCell ref="A314:A319"/>
+    <mergeCell ref="A320:A325"/>
+    <mergeCell ref="A218:A223"/>
+    <mergeCell ref="A224:A229"/>
+    <mergeCell ref="A230:A235"/>
+    <mergeCell ref="A236:A241"/>
+    <mergeCell ref="A242:A247"/>
+    <mergeCell ref="A248:A253"/>
+    <mergeCell ref="A254:A259"/>
+    <mergeCell ref="A260:A265"/>
+    <mergeCell ref="A266:A271"/>
+    <mergeCell ref="A164:A169"/>
+    <mergeCell ref="A170:A175"/>
+    <mergeCell ref="A176:A181"/>
+    <mergeCell ref="A182:A187"/>
+    <mergeCell ref="A188:A193"/>
+    <mergeCell ref="A194:A199"/>
+    <mergeCell ref="A200:A205"/>
+    <mergeCell ref="A206:A211"/>
+    <mergeCell ref="A212:A217"/>
+    <mergeCell ref="A109:A121"/>
+    <mergeCell ref="A31:A40"/>
+    <mergeCell ref="A122:A127"/>
+    <mergeCell ref="A128:A133"/>
+    <mergeCell ref="A134:A139"/>
+    <mergeCell ref="A140:A145"/>
+    <mergeCell ref="A146:A151"/>
+    <mergeCell ref="A152:A157"/>
+    <mergeCell ref="A158:A163"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L30" r:id="rId1" xr:uid="{0B00E541-600E-124F-8530-7CF03623D698}"/>
@@ -38331,7 +38336,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E33" ca="1" si="0">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>81087480</v>
+        <v>214773416</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -38349,7 +38354,7 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>112265433</v>
+        <v>181448040</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -38367,7 +38372,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>117249702</v>
+        <v>71428560</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -38385,7 +38390,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>126606315</v>
+        <v>117569794</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -38403,7 +38408,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>179135370</v>
+        <v>111539475</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -38421,7 +38426,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>74805200</v>
+        <v>53781268</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -38439,7 +38444,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>129074175</v>
+        <v>84412300</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -38457,7 +38462,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>157405392</v>
+        <v>150935750</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -38475,7 +38480,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>75973359</v>
+        <v>134773100</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -38493,7 +38498,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>135661704</v>
+        <v>81165952</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -38511,7 +38516,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>207311375</v>
+        <v>145745582</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -38529,7 +38534,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>97023943</v>
+        <v>237588897</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -38547,7 +38552,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>179589960</v>
+        <v>151329360</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -38565,7 +38570,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>42747705</v>
+        <v>213215343</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -38583,7 +38588,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>100389822</v>
+        <v>157737645</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -38601,7 +38606,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>67806102</v>
+        <v>104526692</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -38619,7 +38624,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>215023392</v>
+        <v>139210929</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -38637,7 +38642,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>39036690</v>
+        <v>68530541</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -38655,7 +38660,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>62369140</v>
+        <v>71957448</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -38673,7 +38678,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>69701625</v>
+        <v>116403003</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -38691,7 +38696,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>82386003</v>
+        <v>257337938</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -38709,7 +38714,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>131559738</v>
+        <v>83565312</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -38727,7 +38732,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>197649144</v>
+        <v>97831608</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -38745,7 +38750,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>100031974</v>
+        <v>182844158</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -38763,7 +38768,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>160754400</v>
+        <v>142826838</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -38781,7 +38786,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>255884598</v>
+        <v>184974760</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -38799,7 +38804,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>72696925</v>
+        <v>171511230</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -38817,7 +38822,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>154218672</v>
+        <v>187365165</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -38835,7 +38840,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>180224850</v>
+        <v>108576174</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -38853,7 +38858,7 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>255741736</v>
+        <v>79142650</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -38871,7 +38876,7 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>134934680</v>
+        <v>101499200</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -38889,7 +38894,7 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>51710876</v>
+        <v>182797020</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -38907,7 +38912,7 @@
       </c>
       <c r="E34">
         <f t="shared" ref="E34:E65" ca="1" si="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>149767044</v>
+        <v>110499252</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -38925,7 +38930,7 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="1"/>
-        <v>198627960</v>
+        <v>134784594</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -38943,7 +38948,7 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="1"/>
-        <v>112279322</v>
+        <v>120433287</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -38961,7 +38966,7 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="1"/>
-        <v>67701816</v>
+        <v>63694991</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -38979,7 +38984,7 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="1"/>
-        <v>163180000</v>
+        <v>156065148</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -38997,7 +39002,7 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="1"/>
-        <v>177393300</v>
+        <v>51949491</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -39015,7 +39020,7 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="1"/>
-        <v>188820710</v>
+        <v>63458178</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -39033,7 +39038,7 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="1"/>
-        <v>121235566</v>
+        <v>125155090</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -39051,7 +39056,7 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="1"/>
-        <v>77864778</v>
+        <v>98420000</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -39069,7 +39074,7 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="1"/>
-        <v>152636510</v>
+        <v>269815200</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -39087,7 +39092,7 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="1"/>
-        <v>210049539</v>
+        <v>82893216</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -39105,7 +39110,7 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="1"/>
-        <v>134573004</v>
+        <v>218844223</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -39123,7 +39128,7 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="1"/>
-        <v>135400925</v>
+        <v>119512080</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -39141,7 +39146,7 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="1"/>
-        <v>165284250</v>
+        <v>121469770</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -39159,7 +39164,7 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="1"/>
-        <v>72108344</v>
+        <v>124822296</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -39177,7 +39182,7 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="1"/>
-        <v>136020586</v>
+        <v>55363375</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -39195,7 +39200,7 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="1"/>
-        <v>271632165</v>
+        <v>60626889</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -39213,7 +39218,7 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="1"/>
-        <v>113308910</v>
+        <v>57269252</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -39231,7 +39236,7 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="1"/>
-        <v>144239708</v>
+        <v>172821528</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -39249,7 +39254,7 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="1"/>
-        <v>143154416</v>
+        <v>152698770</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -39267,7 +39272,7 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="1"/>
-        <v>91874328</v>
+        <v>48523690</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -39285,7 +39290,7 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="1"/>
-        <v>133081828</v>
+        <v>171749925</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -39303,7 +39308,7 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="1"/>
-        <v>118653352</v>
+        <v>200687650</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -39321,7 +39326,7 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="1"/>
-        <v>60013602</v>
+        <v>112351254</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -39339,7 +39344,7 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="1"/>
-        <v>79665033</v>
+        <v>129956785</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -39357,7 +39362,7 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="1"/>
-        <v>227914605</v>
+        <v>98396130</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -39375,7 +39380,7 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="1"/>
-        <v>183497562</v>
+        <v>124050544</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -39393,7 +39398,7 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="1"/>
-        <v>62793599</v>
+        <v>96211500</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -39411,7 +39416,7 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="1"/>
-        <v>139925879</v>
+        <v>153990564</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -39429,7 +39434,7 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="1"/>
-        <v>77345325</v>
+        <v>175511518</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -39447,7 +39452,7 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="1"/>
-        <v>166551042</v>
+        <v>83718432</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -39465,7 +39470,7 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="1"/>
-        <v>160077540</v>
+        <v>103349929</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -39483,7 +39488,7 @@
       </c>
       <c r="E66">
         <f t="shared" ref="E66:E77" ca="1" si="2">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>190451850</v>
+        <v>178682819</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -39501,7 +39506,7 @@
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="2"/>
-        <v>184210377</v>
+        <v>109476846</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -39519,7 +39524,7 @@
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="2"/>
-        <v>155987703</v>
+        <v>139921008</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -39537,7 +39542,7 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="2"/>
-        <v>208503416</v>
+        <v>120378501</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -39555,7 +39560,7 @@
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="2"/>
-        <v>201342240</v>
+        <v>201029192</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -39573,7 +39578,7 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="2"/>
-        <v>259699404</v>
+        <v>158919820</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -39591,7 +39596,7 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="2"/>
-        <v>83379736</v>
+        <v>171693620</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -39609,7 +39614,7 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="2"/>
-        <v>233655114</v>
+        <v>112368300</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -39627,7 +39632,7 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="2"/>
-        <v>85161582</v>
+        <v>229073405</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -39645,7 +39650,7 @@
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="2"/>
-        <v>51761984</v>
+        <v>205970452</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -39663,7 +39668,7 @@
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="2"/>
-        <v>118616724</v>
+        <v>60436806</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -39681,7 +39686,7 @@
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="2"/>
-        <v>128109600</v>
+        <v>112306194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>